<commit_message>
add & upd opt
</commit_message>
<xml_diff>
--- a/opt2019/files/opt.xlsx
+++ b/opt2019/files/opt.xlsx
@@ -1735,7 +1735,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1888,7 +1888,7 @@
         <v>80</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" t="s">
         <v>47</v>
@@ -1956,7 +1956,7 @@
         <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
@@ -2058,7 +2058,7 @@
         <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
         <v>44</v>
@@ -2075,7 +2075,7 @@
         <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -2092,7 +2092,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s">
         <v>54</v>
@@ -2126,7 +2126,7 @@
         <v>55</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" t="s">
         <v>42</v>
@@ -2143,7 +2143,7 @@
         <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" t="s">
         <v>38</v>

</xml_diff>